<commit_message>
Minor updates to scoping review data for resubmission
</commit_message>
<xml_diff>
--- a/sim_scoping_data_full.xlsx
+++ b/sim_scoping_data_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theaknowles/Documents/GitHub/Speech-In-Masks_scoping_review/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thea/Library/CloudStorage/GoogleDrive-thea@msu.edu/.shortcut-targets-by-id/13YgdixLu6IHXjMJ0mgYyj-0HKPxjSRhk/CASALab/1_Projects/SiM/sim_scoping_review_files/revision1_2022-12-01/submission_2022-03-29/tbls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E63345-93E1-4E41-82F1-1D69DD2BDE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68640127-EC9C-B04B-90AA-16E27AAE0348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="47820" windowHeight="25540" xr2:uid="{9FC31C68-FDD9-F644-A918-481620D03B4B}"/>
+    <workbookView xWindow="860" yWindow="500" windowWidth="37540" windowHeight="20180" xr2:uid="{9FC31C68-FDD9-F644-A918-481620D03B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Acoustic-Perceptual-FOR-PUBLICA" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -716,14 +717,6 @@
 N95: peak attenuation of ~10 dB at 800 Hz and 2 kHz - 3 kHz</t>
   </si>
   <si>
-    <t>Greater accuracy for no mask compared to all 3 mask conditions, with greatest detriment from N95.
-Surgical and cloth mask &gt; N95, but did not differ from each other
-No mask: 79.1%; surgical: 69.8%; cloth: 70.8%, N95: 63.2%
-No interaction between condition, speaker
-Non-responses (rather than phonetic approximations): greater for N95 compared to surgical, cloth (which did not differ from each other): 
-surgical: 36.9%, cloth: 37.7%, n95: 44.1%</t>
-  </si>
-  <si>
     <t>n= 8; 5 half-mask FFP of different styles (2 overlaid with surgical mask), 1 surgical mask, 1 half-mask elastomeric, 1 hooded powered air purifying respirator</t>
   </si>
   <si>
@@ -996,12 +989,20 @@
 Lowest intelligibility for elastomeric respirator compared to the average of the other 7 (72% vs 85%)
 Cup-shaped N95 w/ exhalation valve + surgical mask overlaid had lower intelligibility than: 1) n95 without exhalation valve and without overlaid SM, 2) no device. No other significant differences across masks of interest in this review. </t>
   </si>
+  <si>
+    <t>Greater accuracy for no mask compared to all 3 mask conditions, with greatest detriment from N95.
+Surgical and cloth mask &lt; N95, but did not differ from each other
+No mask: 79.1%; surgical: 69.8%; cloth: 70.8%, N95: 63.2%
+No interaction between condition, speaker
+Non-responses (rather than phonetic approximations): greater for N95 compared to surgical, cloth (which did not differ from each other): 
+surgical: 36.9%, cloth: 37.7%, n95: 44.1%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1060,6 +1061,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1124,7 +1132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1185,6 +1193,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1522,7 +1533,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.19921875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2020,10 +2031,10 @@
       <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="2">
         <v>2021</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -2781,10 +2792,10 @@
       <c r="G16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="24" t="s">
         <v>99</v>
       </c>
       <c r="J16" s="2">
@@ -2864,10 +2875,10 @@
       <c r="G17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="23" t="s">
         <v>29</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -2947,10 +2958,10 @@
       <c r="G18" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="23" t="s">
         <v>108</v>
       </c>
       <c r="J18" s="2">
@@ -3030,10 +3041,10 @@
       <c r="G19" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="23" t="s">
         <v>29</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -3112,10 +3123,10 @@
       <c r="G20" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="I20" s="23" t="s">
         <v>29</v>
       </c>
       <c r="J20" s="2">
@@ -3195,10 +3206,10 @@
       <c r="G21" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="23" t="s">
         <v>29</v>
       </c>
       <c r="J21" s="2">
@@ -3278,10 +3289,10 @@
       <c r="G22" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="I22" s="26" t="s">
         <v>131</v>
       </c>
       <c r="J22" s="14">
@@ -3361,10 +3372,10 @@
       <c r="G23" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="H23" s="24" t="s">
+      <c r="H23" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="I23" s="16" t="s">
         <v>137</v>
       </c>
       <c r="J23" s="16">
@@ -3444,10 +3455,10 @@
       <c r="G24" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="J24" s="2">
@@ -3487,7 +3498,7 @@
         <v>29</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
@@ -3527,10 +3538,10 @@
       <c r="G25" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="I25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="J25" s="2">
@@ -3568,7 +3579,7 @@
       </c>
       <c r="U25" s="2"/>
       <c r="V25" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
@@ -3606,10 +3617,10 @@
       <c r="G26" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H26" s="22" t="s">
+      <c r="H26" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="I26" s="23" t="s">
         <v>154</v>
       </c>
       <c r="J26" s="2">
@@ -3689,10 +3700,10 @@
       <c r="G27" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="16" t="s">
         <v>29</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -3772,10 +3783,10 @@
       <c r="G28" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="16" t="s">
         <v>164</v>
       </c>
       <c r="J28" s="2">
@@ -3959,8 +3970,8 @@
       <c r="N30" s="2">
         <v>0</v>
       </c>
-      <c r="O30" s="2" t="s">
-        <v>175</v>
+      <c r="O30" s="22" t="s">
+        <v>250</v>
       </c>
       <c r="P30" s="13">
         <v>0</v>
@@ -4008,16 +4019,16 @@
         <v>2010</v>
       </c>
       <c r="D31" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="F31" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="G31" s="16" t="s">
         <v>178</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>179</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>29</v>
@@ -4041,7 +4052,7 @@
         <v>29</v>
       </c>
       <c r="O31" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P31" s="13">
         <v>0</v>
@@ -4062,7 +4073,7 @@
         <v>29</v>
       </c>
       <c r="V31" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="W31" s="16"/>
       <c r="X31" s="16"/>
@@ -4091,16 +4102,16 @@
         <v>2020</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>29</v>
@@ -4124,7 +4135,7 @@
         <v>29</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P32" s="13">
         <v>0</v>
@@ -4145,7 +4156,7 @@
         <v>29</v>
       </c>
       <c r="V32" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
@@ -4168,25 +4179,25 @@
         <v>Saeidi et al.,  2016</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C33" s="16">
         <v>2016</v>
       </c>
       <c r="D33" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="E33" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>188</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>29</v>
       </c>
       <c r="G33" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="H33" s="16" t="s">
         <v>189</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>190</v>
       </c>
       <c r="I33" s="16" t="s">
         <v>29</v>
@@ -4207,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P33" s="13">
         <v>0</v>
@@ -4255,22 +4266,22 @@
         <v>2017</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H34" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="I34" s="12" t="s">
         <v>195</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>196</v>
       </c>
       <c r="J34" s="12">
         <v>0</v>
@@ -4338,19 +4349,19 @@
         <v>2021</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="12" t="s">
         <v>200</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>201</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>29</v>
@@ -4371,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P35" s="13">
         <v>1</v>
@@ -4392,7 +4403,7 @@
         <v>29</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="W35" s="2"/>
       <c r="X35" s="2"/>
@@ -4421,19 +4432,19 @@
         <v>2021</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" s="12" t="s">
         <v>206</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>207</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>29</v>
@@ -4454,7 +4465,7 @@
         <v>0</v>
       </c>
       <c r="O36" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P36" s="13">
         <v>0</v>
@@ -4504,16 +4515,16 @@
         <v>2021</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="12" t="s">
         <v>211</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>212</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>29</v>
@@ -4537,7 +4548,7 @@
         <v>29</v>
       </c>
       <c r="O37" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P37" s="13">
         <v>1</v>
@@ -4558,7 +4569,7 @@
         <v>29</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W37" s="2"/>
       <c r="X37" s="2"/>
@@ -4577,7 +4588,7 @@
     </row>
     <row r="38" spans="1:36" ht="90" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>38</v>
@@ -4586,19 +4597,19 @@
         <v>2021</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="12" t="s">
         <v>219</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>220</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>29</v>
@@ -4619,7 +4630,7 @@
         <v>0</v>
       </c>
       <c r="O38" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P38" s="13">
         <v>0</v>
@@ -4640,7 +4651,7 @@
         <v>29</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="W38" s="2"/>
       <c r="X38" s="2"/>
@@ -4669,16 +4680,16 @@
         <v>2013</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>29</v>
@@ -4702,7 +4713,7 @@
         <v>29</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P39" s="13">
         <v>0</v>
@@ -4720,10 +4731,10 @@
         <v>0</v>
       </c>
       <c r="U39" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="V39" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="V39" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="W39" s="2"/>
       <c r="X39" s="2"/>
@@ -4752,19 +4763,19 @@
         <v>2020</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G40" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H40" s="14" t="s">
         <v>232</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>233</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>29</v>
@@ -4806,7 +4817,7 @@
         <v>29</v>
       </c>
       <c r="V40" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
@@ -4825,7 +4836,7 @@
     </row>
     <row r="41" spans="1:36" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>26</v>
@@ -4834,19 +4845,19 @@
         <v>2020</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G41" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>29</v>
@@ -4907,7 +4918,7 @@
     </row>
     <row r="42" spans="1:36" ht="150" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>53</v>
@@ -4916,16 +4927,16 @@
         <v>2011</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>29</v>
@@ -4949,7 +4960,7 @@
         <v>29</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P42" s="13">
         <v>0</v>
@@ -4967,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="U42" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V42" s="2" t="s">
         <v>29</v>

</xml_diff>